<commit_message>
Updated pricing document w/ variants
</commit_message>
<xml_diff>
--- a/bom/ovrBeacon_pricing.xlsx
+++ b/bom/ovrBeacon_pricing.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4520" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-4520" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ovrBeaconGateway-wifi_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Stock" sheetId="3" r:id="rId1"/>
+    <sheet name="Variant - No Accelerometer" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="104">
   <si>
     <t>Reference</t>
   </si>
@@ -411,7 +412,25 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -441,6 +460,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:J32" totalsRowCount="1">
+  <autoFilter ref="A1:J31"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Reference"/>
+    <tableColumn id="2" name="Manufacturer"/>
+    <tableColumn id="3" name="Man. Part Num."/>
+    <tableColumn id="4" name="Supplier"/>
+    <tableColumn id="5" name="Supplier Part Num."/>
+    <tableColumn id="6" name="Quantity"/>
+    <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="6" dataCellStyle="Currency">
+      <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
+      <totalsRowFormula>SUM(H2:H31)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Price (qty 1000)" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Currency">
+      <calculatedColumnFormula>F2*I2</calculatedColumnFormula>
+      <totalsRowFormula>SUM(J2:J31)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J32" totalsRowCount="1">
   <autoFilter ref="A1:J31"/>
   <tableColumns count="10">
@@ -450,13 +494,13 @@
     <tableColumn id="4" name="Supplier"/>
     <tableColumn id="5" name="Supplier Part Num."/>
     <tableColumn id="6" name="Quantity"/>
-    <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
       <totalsRowFormula>SUM(H2:H31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Price (qty 1000)" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="8" name="Price (qty 1000)" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*I2</calculatedColumnFormula>
       <totalsRowFormula>SUM(J2:J31)</totalsRowFormula>
     </tableColumn>
@@ -733,6 +777,1008 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>11.49</v>
+      </c>
+      <c r="H2" s="1">
+        <f>F2*G2</f>
+        <v>11.49</v>
+      </c>
+      <c r="I2" s="3">
+        <v>6.9488500000000002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>F2*I2</f>
+        <v>6.9488500000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H26" si="0">F3*G3</f>
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3.6099999999999999E-3</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J26" si="1">F3*I3</f>
+        <v>1.805E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.515E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.515E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>8.8199999999999997E-3</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>8.8199999999999997E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1520000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.7779999999999999E-2</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5559999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.545E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>3.09E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.18725</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.18725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.33E-3</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
+        <v>2.33E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.33E-3</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>4.6600000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.33E-3</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="1"/>
+        <v>2.33E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.0830000000000001E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="1"/>
+        <v>4.1660000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>4.7299999999999998E-3</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>9.4599999999999997E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I15" s="3">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33239999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>5.5399999999999998E-3</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5399999999999998E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5.5399999999999998E-3</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5399999999999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.48</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.44219999999999998</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.88439999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3.39</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>3.39</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.6950000000000001</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6950000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2.1168</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.35102</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.35102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.91</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.94091000000000002</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="1"/>
+        <v>0.94091000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.43106</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.43106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7.86</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>7.86</v>
+      </c>
+      <c r="I24" s="3">
+        <v>4.45946</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="1"/>
+        <v>4.45946</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.33099000000000001</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33099000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.93930000000000002</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="1"/>
+        <v>0.93930000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" ref="H30" si="2">F30*G30</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" ref="J30:J31" si="3">F30*I30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="3">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="2">
+        <f>SUM(H2:H31)</f>
+        <v>38.809999999999995</v>
+      </c>
+      <c r="J32" s="2">
+        <f>SUM(J2:J31)</f>
+        <v>22.828959999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri Bold,Bold"&amp;K000000ovrBeacon
+&amp;A&amp;R&amp;"Calibri Bold,Bold"&amp;K00000026-February-2017_x000D_ Hardware v0.3</oddHeader>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J32"/>
+  <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
@@ -1548,21 +2594,21 @@
         <v>101</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>7.86</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="0"/>
-        <v>7.86</v>
+        <v>0</v>
       </c>
       <c r="I24" s="3">
         <v>4.45946</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="1"/>
-        <v>4.45946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1702,11 +2748,11 @@
       </c>
       <c r="H32" s="2">
         <f>SUM(H2:H31)</f>
-        <v>38.809999999999995</v>
+        <v>30.949999999999996</v>
       </c>
       <c r="J32" s="2">
         <f>SUM(J2:J31)</f>
-        <v>22.828959999999999</v>
+        <v>18.369499999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1714,7 +2760,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"-,Bold"ovrBeacon&amp;R&amp;"-,Bold"_x000D_26-February-2017_x000D_ Hardware v0.3</oddHeader>
+    <oddHeader>&amp;C&amp;"Calibri Bold,Bold"&amp;K000000ovrBeacon
+&amp;A&amp;R&amp;"Calibri Bold,Bold"&amp;K00000026-February-2017_x000D_ Hardware v0.3</oddHeader>
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>